<commit_message>
xin chao cac ban
</commit_message>
<xml_diff>
--- a/QuanTriRuiRoFx.xlsx
+++ b/QuanTriRuiRoFx.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="105">
   <si>
     <t>Nội dung</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>Mỗi người nên tự tạo ra bản kế hoạch trade cho riêng mình</t>
+  </si>
+  <si>
+    <t>https://github.com/thangbk236/QuanTriFx</t>
   </si>
 </sst>
 </file>
@@ -724,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,6 +775,9 @@
       <c r="A6" s="3" t="s">
         <v>77</v>
       </c>
+      <c r="H6" s="3" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">

</xml_diff>

<commit_message>
bo xung ban phan tich gbpusd
</commit_message>
<xml_diff>
--- a/QuanTriRuiRoFx.xlsx
+++ b/QuanTriRuiRoFx.xlsx
@@ -312,9 +312,6 @@
     <t>Sử dụng bollinger band hoặc ma để xác định hội tụ</t>
   </si>
   <si>
-    <t>Thiên Yết</t>
-  </si>
-  <si>
     <t>Người thực hiện:</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>https://github.com/thangbk236/QuanTriFx</t>
+  </si>
+  <si>
+    <t>thangbk236</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,7 @@
   <dimension ref="A1:P96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,23 +746,23 @@
   <sheetData>
     <row r="1" spans="1:8" ht="90" x14ac:dyDescent="1.1499999999999999">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -776,17 +776,17 @@
         <v>77</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -904,7 +904,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D34" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>28</v>
@@ -1258,12 +1258,12 @@
         <v>78</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J78" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="3:16" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
     </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F89" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>